<commit_message>
Fase 2: Diseño: upload
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de documentacion/planilla gantt - escala de tiempo.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de documentacion/planilla gantt - escala de tiempo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b45cdc74189cdafe/DUOCUC/CAPSTONE/PROYECTO/Fase 2/Documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matad\Documents\GitHub\Documentos-CAPSTONE\Fase 2\Evidencias Proyecto\Evidencias de documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D7900D2E-8F74-4D49-869F-4CF60F3522AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D3E8AD6-6901-4C90-8266-3E2142036472}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE65525-802C-42E1-8BF7-4F06489B6F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-12660" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="- AYUDA -" sheetId="2" r:id="rId1"/>
@@ -71,13 +71,13 @@
     <t>Kick Off</t>
   </si>
   <si>
-    <t>Definicion y Analisis requerimientos</t>
-  </si>
-  <si>
     <t>Desarrollo de proyecto</t>
   </si>
   <si>
     <t>Monitoreo producto final  / Cierre de proyecto</t>
+  </si>
+  <si>
+    <t>Definicion y Analisis requerimientos, Diseño</t>
   </si>
 </sst>
 </file>
@@ -1718,8 +1718,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B1:DE32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D12" s="15">
         <v>45901</v>
@@ -3088,7 +3088,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="15">
         <v>45922</v>
@@ -3207,7 +3207,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="15">
         <v>45967</v>

</xml_diff>